<commit_message>
them ho ten va ngay thang cho check list
</commit_message>
<xml_diff>
--- a/security/checklist_security-lab3.xlsx
+++ b/security/checklist_security-lab3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chuyendephattrienweb1_2024\security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7CDB32-9A2D-4611-A8DB-DF73F0651693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2E8194-9CB6-47A7-B2D0-B19D527292F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Tên project</t>
   </si>
@@ -116,9 +116,6 @@
 - Thêm mới thành công
 - Tìm kiếm thành công
 Nếu thỏa là OK</t>
-  </si>
-  <si>
-    <t>SV</t>
   </si>
   <si>
     <t>Câu 2:
@@ -466,13 +463,16 @@
   <si>
     <t>NG</t>
   </si>
+  <si>
+    <t>Xuân Nghĩa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy\-mmm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mmm\-dd"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -782,20 +782,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -813,6 +801,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1274,8 +1274,8 @@
   <dimension ref="A1:AE898"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X12" sqref="X12"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1290,38 +1290,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="24.6" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="31"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="37"/>
       <c r="AE1" s="12"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" ht="13.2">
@@ -1337,71 +1337,71 @@
     </row>
     <row r="3" spans="1:31" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="32" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="33" t="s">
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="33"/>
-      <c r="AC3" s="33"/>
-      <c r="AD3" s="38" t="str">
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="34" t="str">
         <f>"Point: "&amp;SUM(AD5:AD13)</f>
         <v>Point: 8</v>
       </c>
       <c r="AE3" s="12"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
-      <c r="B4" s="37"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
       <c r="X4" s="10" t="s">
         <v>20</v>
       </c>
@@ -1420,44 +1420,44 @@
       <c r="AC4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD4" s="38"/>
+      <c r="AD4" s="34"/>
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="1:31" ht="133.94999999999999" customHeight="1">
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
       <c r="X5" s="11">
         <v>45568</v>
       </c>
       <c r="Y5" s="16" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="Z5" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA5" s="16"/>
       <c r="AB5" s="16"/>
@@ -1473,33 +1473,37 @@
         <f t="shared" ref="B6:B28" si="0">B5+1</f>
         <v>2</v>
       </c>
-      <c r="C6" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="16"/>
+      <c r="C6" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y6" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z6" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA6" s="16"/>
       <c r="AB6" s="16"/>
@@ -1515,33 +1519,37 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="16"/>
+      <c r="C7" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y7" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z7" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA7" s="16"/>
       <c r="AB7" s="16"/>
@@ -1557,39 +1565,43 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="16"/>
+      <c r="C8" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y8" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z8" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA8" s="16"/>
       <c r="AB8" s="16"/>
       <c r="AC8" s="16"/>
       <c r="AD8" s="17">
-        <f t="shared" ref="AD7:AD13" si="1">IF(Z8="OK",1,0)</f>
+        <f t="shared" ref="AD8:AD13" si="1">IF(Z8="OK",1,0)</f>
         <v>1</v>
       </c>
       <c r="AE8" s="12"/>
@@ -1598,33 +1610,37 @@
       <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="16"/>
+      <c r="C9" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y9" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z9" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA9" s="16"/>
       <c r="AB9" s="16"/>
@@ -1640,33 +1656,37 @@
         <f>B9+1</f>
         <v>6</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="16"/>
+      <c r="C10" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y10" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z10" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA10" s="16"/>
       <c r="AB10" s="16"/>
@@ -1682,33 +1702,37 @@
         <f>B10+1</f>
         <v>7</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="16"/>
+      <c r="C11" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y11" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z11" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
@@ -1724,33 +1748,37 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C12" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="16"/>
+      <c r="C12" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y12" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z12" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA12" s="16"/>
       <c r="AB12" s="16"/>
@@ -1766,33 +1794,37 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C13" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="16"/>
+      <c r="C13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="11">
+        <v>45568</v>
+      </c>
+      <c r="Y13" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="Z13" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA13" s="16"/>
       <c r="AB13" s="16"/>
@@ -1808,27 +1840,27 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
       <c r="X14" s="11"/>
       <c r="Y14" s="16"/>
       <c r="Z14" s="16"/>
@@ -1843,27 +1875,27 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
       <c r="X15" s="11"/>
       <c r="Y15" s="16"/>
       <c r="Z15" s="16"/>
@@ -1878,27 +1910,27 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
       <c r="X16" s="11"/>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -1913,27 +1945,27 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
       <c r="X17" s="11"/>
       <c r="Y17" s="16"/>
       <c r="Z17" s="16"/>
@@ -1948,27 +1980,27 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
       <c r="X18" s="11"/>
       <c r="Y18" s="16"/>
       <c r="Z18" s="16"/>
@@ -1983,27 +2015,27 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
       <c r="X19" s="11"/>
       <c r="Y19" s="16"/>
       <c r="Z19" s="16"/>
@@ -2018,27 +2050,27 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
       <c r="X20" s="11"/>
       <c r="Y20" s="16"/>
       <c r="Z20" s="16"/>
@@ -2053,27 +2085,27 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
       <c r="X21" s="11"/>
       <c r="Y21" s="16"/>
       <c r="Z21" s="16"/>
@@ -2088,27 +2120,27 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
       <c r="X22" s="11"/>
       <c r="Y22" s="16"/>
       <c r="Z22" s="16"/>
@@ -2123,27 +2155,27 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
       <c r="X23" s="11"/>
       <c r="Y23" s="16"/>
       <c r="Z23" s="16"/>
@@ -2158,27 +2190,27 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
       <c r="X24" s="11"/>
       <c r="Y24" s="16"/>
       <c r="Z24" s="16"/>
@@ -2193,27 +2225,27 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="35"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="31"/>
+      <c r="W25" s="31"/>
       <c r="X25" s="11"/>
       <c r="Y25" s="16"/>
       <c r="Z25" s="16"/>
@@ -2228,27 +2260,27 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="35"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="35"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
       <c r="X26" s="11"/>
       <c r="Y26" s="16"/>
       <c r="Z26" s="16"/>
@@ -2263,27 +2295,27 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
-      <c r="R27" s="35"/>
-      <c r="S27" s="35"/>
-      <c r="T27" s="35"/>
-      <c r="U27" s="35"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="35"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
       <c r="X27" s="11"/>
       <c r="Y27" s="16"/>
       <c r="Z27" s="16"/>
@@ -2298,27 +2330,27 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
       <c r="X28" s="11"/>
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
@@ -4940,6 +4972,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AA3:AC3"/>
+    <mergeCell ref="C5:W5"/>
+    <mergeCell ref="C6:W6"/>
+    <mergeCell ref="C13:W13"/>
+    <mergeCell ref="C14:W14"/>
+    <mergeCell ref="C15:W15"/>
+    <mergeCell ref="C16:W16"/>
+    <mergeCell ref="C7:W7"/>
+    <mergeCell ref="C8:W8"/>
+    <mergeCell ref="C9:W9"/>
+    <mergeCell ref="C10:W10"/>
+    <mergeCell ref="C11:W11"/>
     <mergeCell ref="C27:W27"/>
     <mergeCell ref="C28:W28"/>
     <mergeCell ref="B3:B4"/>
@@ -4956,20 +5002,6 @@
     <mergeCell ref="C20:W20"/>
     <mergeCell ref="C21:W21"/>
     <mergeCell ref="C12:W12"/>
-    <mergeCell ref="C13:W13"/>
-    <mergeCell ref="C14:W14"/>
-    <mergeCell ref="C15:W15"/>
-    <mergeCell ref="C16:W16"/>
-    <mergeCell ref="C7:W7"/>
-    <mergeCell ref="C8:W8"/>
-    <mergeCell ref="C9:W9"/>
-    <mergeCell ref="C10:W10"/>
-    <mergeCell ref="C11:W11"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="C5:W5"/>
-    <mergeCell ref="C6:W6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z5:Z28 AC5:AC28" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>